<commit_message>
added function to simulate market baskets based on rating plan inputs
</commit_message>
<xml_diff>
--- a/examples/Metromile/Metromile policies.xlsx
+++ b/examples/Metromile/Metromile policies.xlsx
@@ -133,118 +133,118 @@
     <t xml:space="preserve">homeowner_at_init</t>
   </si>
   <si>
+    <t xml:space="preserve">full_coverage_code</t>
+  </si>
+  <si>
+    <t xml:space="preserve">min_count</t>
+  </si>
+  <si>
+    <t xml:space="preserve">vehicle_count_at_init</t>
+  </si>
+  <si>
+    <t xml:space="preserve">LOAN_limit</t>
+  </si>
+  <si>
+    <t xml:space="preserve">naf_count</t>
+  </si>
+  <si>
+    <t xml:space="preserve">tenure</t>
+  </si>
+  <si>
+    <t xml:space="preserve">RENT_limit</t>
+  </si>
+  <si>
+    <t xml:space="preserve">spd_count</t>
+  </si>
+  <si>
+    <t xml:space="preserve">prior_insurance_code</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ROAD_limit</t>
+  </si>
+  <si>
+    <t xml:space="preserve">clean_driver</t>
+  </si>
+  <si>
+    <t xml:space="preserve">prior_insurance_level</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ACPE_limit</t>
+  </si>
+  <si>
+    <t xml:space="preserve">prior_bi_code</t>
+  </si>
+  <si>
+    <t xml:space="preserve">EXTMED_limit</t>
+  </si>
+  <si>
+    <t xml:space="preserve">tier</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ESSSRV_limit</t>
+  </si>
+  <si>
+    <t xml:space="preserve">continuous_insurance_discount_level</t>
+  </si>
+  <si>
+    <t xml:space="preserve">DEATH_limit</t>
+  </si>
+  <si>
+    <t xml:space="preserve">silver_continuous_insurance_discount_at_init</t>
+  </si>
+  <si>
+    <t xml:space="preserve">FUNERAL_limit</t>
+  </si>
+  <si>
+    <t xml:space="preserve">gold_continuous_insurance_discount_at_init</t>
+  </si>
+  <si>
+    <t xml:space="preserve">funeral_coverage_group</t>
+  </si>
+  <si>
+    <t xml:space="preserve">BI_limit</t>
+  </si>
+  <si>
+    <t xml:space="preserve">IL_limit</t>
+  </si>
+  <si>
+    <t xml:space="preserve">limitation_on_lawsuits</t>
+  </si>
+  <si>
+    <t xml:space="preserve">COMP_deductible</t>
+  </si>
+  <si>
+    <t xml:space="preserve">PD_limit</t>
+  </si>
+  <si>
+    <t xml:space="preserve">COLL_deductible</t>
+  </si>
+  <si>
+    <t xml:space="preserve">PIP_limit</t>
+  </si>
+  <si>
+    <t xml:space="preserve">PIP_deductible</t>
+  </si>
+  <si>
+    <t xml:space="preserve">UMUIM_limit</t>
+  </si>
+  <si>
+    <t xml:space="preserve">UMPD_limit</t>
+  </si>
+  <si>
+    <t xml:space="preserve">pip_discount</t>
+  </si>
+  <si>
+    <t xml:space="preserve">three_year_safe_driving_discount</t>
+  </si>
+  <si>
+    <t xml:space="preserve">nb_five_year_accident_free</t>
+  </si>
+  <si>
+    <t xml:space="preserve">five_year_claim_free</t>
+  </si>
+  <si>
     <t xml:space="preserve">coverage_group</t>
-  </si>
-  <si>
-    <t xml:space="preserve">min_count</t>
-  </si>
-  <si>
-    <t xml:space="preserve">vehicle_count_at_init</t>
-  </si>
-  <si>
-    <t xml:space="preserve">full_coverage_code</t>
-  </si>
-  <si>
-    <t xml:space="preserve">naf_count</t>
-  </si>
-  <si>
-    <t xml:space="preserve">tenure</t>
-  </si>
-  <si>
-    <t xml:space="preserve">LOAN_limit</t>
-  </si>
-  <si>
-    <t xml:space="preserve">spd_count</t>
-  </si>
-  <si>
-    <t xml:space="preserve">prior_insurance_code</t>
-  </si>
-  <si>
-    <t xml:space="preserve">RENT_limit</t>
-  </si>
-  <si>
-    <t xml:space="preserve">clean_driver</t>
-  </si>
-  <si>
-    <t xml:space="preserve">prior_insurance_level</t>
-  </si>
-  <si>
-    <t xml:space="preserve">ROAD_limit</t>
-  </si>
-  <si>
-    <t xml:space="preserve">prior_bi_code</t>
-  </si>
-  <si>
-    <t xml:space="preserve">ACPE_limit</t>
-  </si>
-  <si>
-    <t xml:space="preserve">tier</t>
-  </si>
-  <si>
-    <t xml:space="preserve">EXTMED_limit</t>
-  </si>
-  <si>
-    <t xml:space="preserve">continuous_insurance_discount_level</t>
-  </si>
-  <si>
-    <t xml:space="preserve">ESSSRV_limit</t>
-  </si>
-  <si>
-    <t xml:space="preserve">silver_continuous_insurance_discount_at_init</t>
-  </si>
-  <si>
-    <t xml:space="preserve">DEATH_limit</t>
-  </si>
-  <si>
-    <t xml:space="preserve">gold_continuous_insurance_discount_at_init</t>
-  </si>
-  <si>
-    <t xml:space="preserve">FUNERAL_limit</t>
-  </si>
-  <si>
-    <t xml:space="preserve">BI_limit</t>
-  </si>
-  <si>
-    <t xml:space="preserve">funeral_coverage_group</t>
-  </si>
-  <si>
-    <t xml:space="preserve">limitation_on_lawsuits</t>
-  </si>
-  <si>
-    <t xml:space="preserve">IL_limit</t>
-  </si>
-  <si>
-    <t xml:space="preserve">PD_limit</t>
-  </si>
-  <si>
-    <t xml:space="preserve">COMP_deductible</t>
-  </si>
-  <si>
-    <t xml:space="preserve">PIP_limit</t>
-  </si>
-  <si>
-    <t xml:space="preserve">COLL_deductible</t>
-  </si>
-  <si>
-    <t xml:space="preserve">PIP_deductible</t>
-  </si>
-  <si>
-    <t xml:space="preserve">UMUIM_limit</t>
-  </si>
-  <si>
-    <t xml:space="preserve">UMPD_limit</t>
-  </si>
-  <si>
-    <t xml:space="preserve">pip_discount</t>
-  </si>
-  <si>
-    <t xml:space="preserve">three_year_safe_driving_discount</t>
-  </si>
-  <si>
-    <t xml:space="preserve">nb_five_year_accident_free</t>
-  </si>
-  <si>
-    <t xml:space="preserve">five_year_claim_free</t>
   </si>
   <si>
     <t xml:space="preserve">pni_marital_status</t>
@@ -295,6 +295,7 @@
       <sz val="10"/>
       <name val="Arial"/>
       <family val="2"/>
+      <charset val="1"/>
     </font>
     <font>
       <sz val="10"/>
@@ -316,6 +317,7 @@
       <sz val="10"/>
       <name val="Arial"/>
       <family val="2"/>
+      <charset val="1"/>
     </font>
   </fonts>
   <fills count="3">
@@ -366,7 +368,7 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="4">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -376,6 +378,10 @@
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="164" fontId="0" fillId="2" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -396,18 +402,18 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:L45"/>
+  <dimension ref="A1:L46"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="110" zoomScaleNormal="110" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="E25" activeCellId="0" sqref="E25"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="D1" colorId="64" zoomScale="120" zoomScaleNormal="120" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="E13" activeCellId="0" sqref="E13"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.55078125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="37.04"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="0" width="17.85"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="0" width="17.86"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="0" width="37.04"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="8" min="8" style="0" width="17.85"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="8" min="8" style="0" width="17.86"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -495,7 +501,7 @@
       <c r="C8" s="0" t="s">
         <v>22</v>
       </c>
-      <c r="E8" s="0" t="s">
+      <c r="E8" s="2" t="s">
         <v>23</v>
       </c>
     </row>
@@ -517,7 +523,7 @@
       <c r="C10" s="0" t="s">
         <v>27</v>
       </c>
-      <c r="E10" s="0" t="s">
+      <c r="E10" s="2" t="s">
         <v>28</v>
       </c>
     </row>
@@ -528,7 +534,7 @@
       <c r="C11" s="0" t="s">
         <v>30</v>
       </c>
-      <c r="E11" s="0" t="s">
+      <c r="E11" s="2" t="s">
         <v>31</v>
       </c>
     </row>
@@ -550,7 +556,7 @@
       <c r="C13" s="0" t="s">
         <v>36</v>
       </c>
-      <c r="E13" s="0" t="s">
+      <c r="E13" s="2" t="s">
         <v>37</v>
       </c>
     </row>
@@ -668,102 +674,104 @@
       <c r="C26" s="0" t="s">
         <v>66</v>
       </c>
-      <c r="E26" s="0" t="s">
-        <v>67</v>
-      </c>
     </row>
     <row r="27" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C27" s="0" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
     </row>
     <row r="28" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C28" s="0" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
     </row>
     <row r="29" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C29" s="0" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="30" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C30" s="2" t="s">
         <v>70</v>
       </c>
     </row>
-    <row r="30" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C30" s="0" t="s">
+    <row r="31" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C31" s="2" t="s">
         <v>71</v>
       </c>
     </row>
-    <row r="31" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C31" s="0" t="s">
+    <row r="32" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C32" s="2" t="s">
         <v>72</v>
       </c>
     </row>
-    <row r="32" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C32" s="0" t="s">
+    <row r="33" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C33" s="2" t="s">
         <v>73</v>
       </c>
     </row>
-    <row r="33" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C33" s="0" t="s">
+    <row r="34" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C34" s="3" t="s">
         <v>74</v>
-      </c>
-    </row>
-    <row r="34" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C34" s="2" t="s">
-        <v>75</v>
       </c>
     </row>
     <row r="35" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C35" s="2" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
     </row>
     <row r="36" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C36" s="2" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
     </row>
     <row r="37" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C37" s="2" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
     </row>
     <row r="38" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C38" s="2" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
     </row>
     <row r="39" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C39" s="2" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
     </row>
     <row r="40" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C40" s="2" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
     </row>
     <row r="41" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C41" s="2" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
     </row>
     <row r="42" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C42" s="2" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
     </row>
     <row r="43" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C43" s="2" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
     </row>
     <row r="44" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C44" s="2" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
     </row>
     <row r="45" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C45" s="2" t="s">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="46" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C46" s="2" t="s">
         <v>86</v>
       </c>
     </row>

</xml_diff>